<commit_message>
changes to plots for report
</commit_message>
<xml_diff>
--- a/cluster_azti/output/Tables.xlsx
+++ b/cluster_azti/output/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495" activeTab="5"/>
+    <workbookView windowWidth="28800" windowHeight="12495" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HCR8" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -307,6 +307,67 @@
     </r>
   </si>
   <si>
+    <t>2041-2050</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1st year P(B1+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Blim) &gt; 95%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1st year P(B1+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Blim_low) &gt; 95%</t>
+    </r>
+  </si>
+  <si>
+    <t>Risk1 for Blim (%)</t>
+  </si>
+  <si>
+    <t>Risk1 for Blim_low (%)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -422,7 +483,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,9 +504,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -445,29 +514,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,7 +544,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,13 +589,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -544,15 +599,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -588,7 +649,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,55 +691,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,37 +703,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,49 +727,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,13 +745,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -940,11 +1001,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -964,41 +1057,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1029,11 +1092,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1042,10 +1103,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1054,13 +1115,13 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1069,7 +1130,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1090,104 +1151,104 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1260,18 +1321,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1295,6 +1350,39 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1697,7 +1785,7 @@
       <c r="J8" s="25"/>
     </row>
     <row r="9" ht="15" spans="2:10">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1712,21 +1800,21 @@
       <c r="F9" s="10">
         <v>326</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="26">
         <v>470</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>468</v>
       </c>
       <c r="I9" s="10">
         <v>423</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="27">
         <v>425</v>
       </c>
     </row>
     <row r="10" ht="15" spans="2:10">
-      <c r="B10" s="29"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="13"/>
       <c r="D10" s="14" t="s">
         <v>12</v>
@@ -1737,21 +1825,21 @@
       <c r="F10" s="3">
         <v>311</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="28">
         <v>509</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="29">
         <v>502</v>
       </c>
       <c r="I10" s="3">
         <v>460</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="29">
         <v>455</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:10">
-      <c r="B11" s="29"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17" t="s">
         <v>13</v>
@@ -1762,21 +1850,21 @@
       <c r="F11" s="18">
         <v>276</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="30">
         <v>565</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="31">
         <v>568</v>
       </c>
       <c r="I11" s="18">
         <v>555</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="31">
         <v>551</v>
       </c>
     </row>
     <row r="12" ht="15" spans="2:10">
-      <c r="B12" s="29"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1789,21 +1877,21 @@
       <c r="F12" s="10">
         <v>0.1</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <v>0.079</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <v>0.08</v>
       </c>
       <c r="I12" s="10">
         <v>0.08</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="27">
         <v>0.082</v>
       </c>
     </row>
     <row r="13" ht="15" spans="2:10">
-      <c r="B13" s="29"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="14" t="s">
         <v>12</v>
@@ -1814,21 +1902,21 @@
       <c r="F13" s="3">
         <v>0.1</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="28">
         <v>0.076</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="29">
         <v>0.077</v>
       </c>
       <c r="I13" s="3">
         <v>0.076</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="29">
         <v>0.08</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="2:10">
-      <c r="B14" s="29"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17" t="s">
         <v>13</v>
@@ -1839,21 +1927,21 @@
       <c r="F14" s="18">
         <v>0.128</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="30">
         <v>0.072</v>
       </c>
-      <c r="H14" s="33">
+      <c r="H14" s="31">
         <v>0.072</v>
       </c>
       <c r="I14" s="18">
         <v>0.072</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="31">
         <v>0.074</v>
       </c>
     </row>
     <row r="15" ht="15" spans="2:10">
-      <c r="B15" s="29"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="8" t="s">
         <v>15</v>
       </c>
@@ -1866,21 +1954,21 @@
       <c r="F15" s="10">
         <v>33</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="26">
         <v>40</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <v>40</v>
       </c>
       <c r="I15" s="10">
         <v>40</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="27">
         <v>40</v>
       </c>
     </row>
     <row r="16" ht="15" spans="2:10">
-      <c r="B16" s="29"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="13"/>
       <c r="D16" s="14" t="s">
         <v>12</v>
@@ -1891,21 +1979,21 @@
       <c r="F16" s="3">
         <v>31</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="28">
         <v>40</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="29">
         <v>40</v>
       </c>
       <c r="I16" s="3">
         <v>40</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="29">
         <v>40</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="2:10">
-      <c r="B17" s="29"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
         <v>13</v>
@@ -1916,21 +2004,21 @@
       <c r="F17" s="18">
         <v>37</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="30">
         <v>40</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H17" s="31">
         <v>40</v>
       </c>
       <c r="I17" s="18">
         <v>40</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="31">
         <v>40</v>
       </c>
     </row>
     <row r="18" ht="15" spans="2:10">
-      <c r="B18" s="29"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -1943,21 +2031,21 @@
       <c r="F18" s="10">
         <v>4</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="26">
         <v>3</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="27">
         <v>3</v>
       </c>
       <c r="I18" s="10">
         <v>4</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="19" ht="15" spans="2:10">
-      <c r="B19" s="29"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="14" t="s">
         <v>12</v>
@@ -1968,21 +2056,21 @@
       <c r="F19" s="3">
         <v>5</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="28">
         <v>2</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H19" s="29">
         <v>2</v>
       </c>
       <c r="I19" s="3">
         <v>3</v>
       </c>
-      <c r="J19" s="31">
+      <c r="J19" s="29">
         <v>3</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="2:10">
-      <c r="B20" s="29"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="16"/>
       <c r="D20" s="17" t="s">
         <v>13</v>
@@ -1993,22 +2081,22 @@
       <c r="F20" s="18">
         <v>4</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="30">
         <v>1</v>
       </c>
-      <c r="H20" s="33">
+      <c r="H20" s="31">
         <v>0</v>
       </c>
       <c r="I20" s="18">
         <v>1</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J20" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="21" ht="15" spans="2:10">
-      <c r="B21" s="29"/>
-      <c r="C21" s="34" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -2020,22 +2108,22 @@
       <c r="F21" s="10">
         <v>0</v>
       </c>
-      <c r="G21" s="27">
-        <v>0</v>
-      </c>
-      <c r="H21" s="28">
+      <c r="G21" s="26">
+        <v>0</v>
+      </c>
+      <c r="H21" s="27">
         <v>0</v>
       </c>
       <c r="I21" s="10">
         <v>0</v>
       </c>
-      <c r="J21" s="28">
+      <c r="J21" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="22" ht="15" spans="2:10">
-      <c r="B22" s="29"/>
-      <c r="C22" s="35"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="14" t="s">
         <v>12</v>
       </c>
@@ -2045,22 +2133,22 @@
       <c r="F22" s="3">
         <v>0</v>
       </c>
-      <c r="G22" s="30">
-        <v>0</v>
-      </c>
-      <c r="H22" s="31">
+      <c r="G22" s="28">
+        <v>0</v>
+      </c>
+      <c r="H22" s="29">
         <v>0</v>
       </c>
       <c r="I22" s="3">
         <v>0</v>
       </c>
-      <c r="J22" s="31">
+      <c r="J22" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="2:10">
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="17" t="s">
         <v>13</v>
       </c>
@@ -2070,16 +2158,16 @@
       <c r="F23" s="18">
         <v>0</v>
       </c>
-      <c r="G23" s="32">
-        <v>0</v>
-      </c>
-      <c r="H23" s="33">
+      <c r="G23" s="30">
+        <v>0</v>
+      </c>
+      <c r="H23" s="31">
         <v>0</v>
       </c>
       <c r="I23" s="18">
         <v>0</v>
       </c>
-      <c r="J23" s="33">
+      <c r="J23" s="31">
         <v>0</v>
       </c>
     </row>
@@ -2099,16 +2187,16 @@
       <c r="F24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="26">
         <v>2024</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="27">
         <v>2025</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J24" s="28" t="s">
+      <c r="J24" s="27" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2126,16 +2214,16 @@
       <c r="F25" s="18">
         <v>2021</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="30">
         <v>2021</v>
       </c>
-      <c r="H25" s="33">
+      <c r="H25" s="31">
         <v>2021</v>
       </c>
       <c r="I25" s="18">
         <v>2021</v>
       </c>
-      <c r="J25" s="33">
+      <c r="J25" s="31">
         <v>2021</v>
       </c>
     </row>
@@ -2153,16 +2241,16 @@
       <c r="F26" s="3">
         <v>85</v>
       </c>
-      <c r="G26" s="30">
+      <c r="G26" s="28">
         <v>2</v>
       </c>
-      <c r="H26" s="31">
+      <c r="H26" s="29">
         <v>2</v>
       </c>
       <c r="I26" s="3">
         <v>7</v>
       </c>
-      <c r="J26" s="31">
+      <c r="J26" s="29">
         <v>9</v>
       </c>
     </row>
@@ -2180,16 +2268,16 @@
       <c r="F27" s="18">
         <v>6</v>
       </c>
-      <c r="G27" s="32">
-        <v>0</v>
-      </c>
-      <c r="H27" s="33">
+      <c r="G27" s="30">
+        <v>0</v>
+      </c>
+      <c r="H27" s="31">
         <v>0</v>
       </c>
       <c r="I27" s="18">
         <v>0</v>
       </c>
-      <c r="J27" s="33">
+      <c r="J27" s="31">
         <v>1</v>
       </c>
     </row>
@@ -2299,7 +2387,7 @@
       <c r="I8" s="25"/>
     </row>
     <row r="9" ht="15" spans="1:9">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -2314,21 +2402,21 @@
       <c r="E9" s="10">
         <v>325</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="26">
         <v>467</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="27">
         <v>464</v>
       </c>
       <c r="H9" s="10">
         <v>421</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="27">
         <v>421</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:9">
-      <c r="A10" s="29"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
         <v>12</v>
@@ -2339,21 +2427,21 @@
       <c r="E10" s="3">
         <v>308</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="28">
         <v>503</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="29">
         <v>496</v>
       </c>
       <c r="H10" s="3">
         <v>455</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="29">
         <v>447</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:9">
-      <c r="A11" s="29"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17" t="s">
         <v>13</v>
@@ -2364,21 +2452,21 @@
       <c r="E11" s="18">
         <v>273</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="30">
         <v>553</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="31">
         <v>559</v>
       </c>
       <c r="H11" s="18">
         <v>540</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="31">
         <v>534</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:9">
-      <c r="A12" s="29"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -2391,21 +2479,21 @@
       <c r="E12" s="10">
         <v>0.104</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="26">
         <v>0.085</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <v>0.087</v>
       </c>
       <c r="H12" s="10">
         <v>0.085</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="27">
         <v>0.089</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:9">
-      <c r="A13" s="29"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14" t="s">
         <v>12</v>
@@ -2416,21 +2504,21 @@
       <c r="E13" s="3">
         <v>0.102</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="28">
         <v>0.084</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="29">
         <v>0.085</v>
       </c>
       <c r="H13" s="3">
         <v>0.082</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="29">
         <v>0.087</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:9">
-      <c r="A14" s="29"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="16"/>
       <c r="C14" s="17" t="s">
         <v>13</v>
@@ -2441,21 +2529,21 @@
       <c r="E14" s="18">
         <v>0.135</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="30">
         <v>0.082</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="31">
         <v>0.082</v>
       </c>
       <c r="H14" s="18">
         <v>0.081</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="31">
         <v>0.084</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:9">
-      <c r="A15" s="29"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
@@ -2468,21 +2556,21 @@
       <c r="E15" s="10">
         <v>33</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="26">
         <v>45</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="27">
         <v>45</v>
       </c>
       <c r="H15" s="10">
         <v>39</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="27">
         <v>43</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:9">
-      <c r="A16" s="29"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14" t="s">
         <v>12</v>
@@ -2493,21 +2581,21 @@
       <c r="E16" s="3">
         <v>30</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="28">
         <v>45</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="29">
         <v>45</v>
       </c>
       <c r="H16" s="3">
         <v>45</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="29">
         <v>45</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="1:9">
-      <c r="A17" s="29"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="16"/>
       <c r="C17" s="17" t="s">
         <v>13</v>
@@ -2518,21 +2606,21 @@
       <c r="E17" s="18">
         <v>36</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="30">
         <v>45</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="31">
         <v>45</v>
       </c>
       <c r="H17" s="18">
         <v>45</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="31">
         <v>45</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:9">
-      <c r="A18" s="29"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
@@ -2545,21 +2633,21 @@
       <c r="E18" s="10">
         <v>6</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="26">
         <v>5</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="27">
         <v>4</v>
       </c>
       <c r="H18" s="10">
         <v>5</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:9">
-      <c r="A19" s="29"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
         <v>12</v>
@@ -2570,21 +2658,21 @@
       <c r="E19" s="3">
         <v>6</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="28">
         <v>3</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="29">
         <v>3</v>
       </c>
       <c r="H19" s="3">
         <v>3</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="29">
         <v>4</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="1:9">
-      <c r="A20" s="29"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="16"/>
       <c r="C20" s="17" t="s">
         <v>13</v>
@@ -2595,22 +2683,22 @@
       <c r="E20" s="18">
         <v>6</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="30">
         <v>1</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="31">
         <v>1</v>
       </c>
       <c r="H20" s="18">
         <v>2</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:9">
-      <c r="A21" s="29"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="32" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -2622,22 +2710,22 @@
       <c r="E21" s="10">
         <v>0</v>
       </c>
-      <c r="F21" s="27">
-        <v>0</v>
-      </c>
-      <c r="G21" s="28">
+      <c r="F21" s="26">
+        <v>0</v>
+      </c>
+      <c r="G21" s="27">
         <v>0</v>
       </c>
       <c r="H21" s="10">
         <v>0</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:9">
-      <c r="A22" s="29"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="14" t="s">
         <v>12</v>
       </c>
@@ -2647,22 +2735,22 @@
       <c r="E22" s="3">
         <v>0</v>
       </c>
-      <c r="F22" s="30">
-        <v>0</v>
-      </c>
-      <c r="G22" s="31">
+      <c r="F22" s="28">
+        <v>0</v>
+      </c>
+      <c r="G22" s="29">
         <v>0</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="1:9">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="17" t="s">
         <v>13</v>
       </c>
@@ -2672,16 +2760,16 @@
       <c r="E23" s="18">
         <v>0</v>
       </c>
-      <c r="F23" s="32">
-        <v>0</v>
-      </c>
-      <c r="G23" s="33">
+      <c r="F23" s="30">
+        <v>0</v>
+      </c>
+      <c r="G23" s="31">
         <v>0</v>
       </c>
       <c r="H23" s="18">
         <v>0</v>
       </c>
-      <c r="I23" s="33">
+      <c r="I23" s="31">
         <v>0</v>
       </c>
     </row>
@@ -2701,16 +2789,16 @@
       <c r="E24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="26">
         <v>2024</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="27">
         <v>2025</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="27" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2728,16 +2816,16 @@
       <c r="E25" s="18">
         <v>2021</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="30">
         <v>2021</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G25" s="31">
         <v>2021</v>
       </c>
       <c r="H25" s="18">
         <v>2021</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I25" s="31">
         <v>2021</v>
       </c>
     </row>
@@ -2755,16 +2843,16 @@
       <c r="E26" s="3">
         <v>86</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="28">
         <v>2</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G26" s="29">
         <v>3</v>
       </c>
       <c r="H26" s="3">
         <v>9</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="29">
         <v>14</v>
       </c>
     </row>
@@ -2782,16 +2870,16 @@
       <c r="E27" s="18">
         <v>6</v>
       </c>
-      <c r="F27" s="32">
-        <v>0</v>
-      </c>
-      <c r="G27" s="33">
+      <c r="F27" s="30">
+        <v>0</v>
+      </c>
+      <c r="G27" s="31">
         <v>0</v>
       </c>
       <c r="H27" s="18">
         <v>0</v>
       </c>
-      <c r="I27" s="33">
+      <c r="I27" s="31">
         <v>1</v>
       </c>
     </row>
@@ -2820,15 +2908,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="41.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="30.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="13.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2838,70 +2926,59 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" ht="13.5"/>
-    <row r="6" ht="15.75" spans="1:9">
+    <row r="6" ht="15.75" spans="1:3">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="25"/>
-    </row>
-    <row r="7" ht="15.75" spans="1:9">
+    </row>
+    <row r="7" ht="15.75" spans="1:12">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="25"/>
+      <c r="L7" s="46"/>
+    </row>
+    <row r="8" ht="15.75" spans="1:12">
+      <c r="A8" s="2"/>
+      <c r="B8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I8" s="25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" ht="15.75" spans="1:9">
-      <c r="A8" s="2"/>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="25"/>
-    </row>
-    <row r="9" ht="15" spans="1:9">
-      <c r="A9" s="26" t="s">
+      <c r="L8" s="46"/>
+    </row>
+    <row r="9" ht="15" spans="1:12">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -2910,509 +2987,1055 @@
       <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="36">
         <v>327</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="37">
         <v>324</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="36">
         <v>465</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="38">
         <v>467</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="37">
         <v>420</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="38">
         <v>421</v>
       </c>
-    </row>
-    <row r="10" ht="15" spans="1:9">
-      <c r="A10" s="29"/>
+      <c r="L9" s="46"/>
+    </row>
+    <row r="10" ht="15" spans="1:12">
+      <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="39">
         <v>315</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="40">
         <v>307</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="39">
         <v>498</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="41">
         <v>496</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="40">
         <v>451</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="41">
         <v>444</v>
       </c>
-    </row>
-    <row r="11" ht="15.75" spans="1:9">
-      <c r="A11" s="29"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17" t="s">
+      <c r="L10" s="46"/>
+    </row>
+    <row r="11" ht="15" spans="1:12">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="39">
+        <v>303</v>
+      </c>
+      <c r="E11" s="40">
+        <v>278</v>
+      </c>
+      <c r="F11" s="39">
+        <v>543</v>
+      </c>
+      <c r="G11" s="41">
+        <v>541</v>
+      </c>
+      <c r="H11" s="40">
+        <v>524</v>
+      </c>
+      <c r="I11" s="41">
+        <v>501</v>
+      </c>
+      <c r="L11" s="46"/>
+    </row>
+    <row r="12" ht="15.75" spans="1:12">
+      <c r="A12" s="12"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D12" s="42">
         <v>302</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E12" s="43">
         <v>271</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F12" s="42">
         <v>542</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G12" s="44">
         <v>542</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H12" s="43">
         <v>527</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I12" s="44">
         <v>510</v>
       </c>
-    </row>
-    <row r="12" ht="15" spans="1:9">
-      <c r="A12" s="29"/>
-      <c r="B12" s="8" t="s">
+      <c r="L12" s="46"/>
+    </row>
+    <row r="13" ht="15" spans="1:12">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D13" s="39">
         <v>0.091</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E13" s="40">
         <v>0.106</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F13" s="39">
         <v>0.091</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G13" s="41">
         <v>0.093</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H13" s="40">
         <v>0.088</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I13" s="41">
         <v>0.094</v>
       </c>
-    </row>
-    <row r="13" ht="15" spans="1:9">
-      <c r="A13" s="29"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14" t="s">
+      <c r="L13" s="46"/>
+    </row>
+    <row r="14" ht="15" spans="1:12">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D14" s="39">
         <v>0.083</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E14" s="40">
         <v>0.103</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F14" s="39">
         <v>0.091</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G14" s="41">
         <v>0.093</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H14" s="40">
         <v>0.087</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I14" s="41">
         <v>0.094</v>
       </c>
-    </row>
-    <row r="14" ht="15.75" spans="1:9">
-      <c r="A14" s="29"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17" t="s">
+      <c r="L14" s="46"/>
+    </row>
+    <row r="15" ht="15" spans="1:12">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="39">
+        <v>0.077</v>
+      </c>
+      <c r="E15" s="40">
+        <v>0.121</v>
+      </c>
+      <c r="F15" s="39">
+        <v>0.091</v>
+      </c>
+      <c r="G15" s="41">
+        <v>0.092</v>
+      </c>
+      <c r="H15" s="40">
+        <v>0.089</v>
+      </c>
+      <c r="I15" s="41">
+        <v>0.094</v>
+      </c>
+      <c r="L15" s="46"/>
+    </row>
+    <row r="16" ht="15.75" spans="1:12">
+      <c r="A16" s="12"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D16" s="39">
         <v>0.076</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E16" s="40">
         <v>0.137</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F16" s="39">
         <v>0.091</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G16" s="41">
         <v>0.093</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H16" s="40">
         <v>0.089</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I16" s="41">
         <v>0.095</v>
       </c>
-    </row>
-    <row r="15" ht="15" spans="1:9">
-      <c r="A15" s="29"/>
-      <c r="B15" s="8" t="s">
+      <c r="L16" s="46"/>
+    </row>
+    <row r="17" ht="15" spans="1:12">
+      <c r="A17" s="12"/>
+      <c r="B17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D17" s="36">
         <v>29</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E17" s="37">
         <v>33</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F17" s="36">
         <v>46</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G17" s="38">
         <v>50</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H17" s="37">
         <v>39</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I17" s="38">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" ht="15" spans="1:9">
-      <c r="A16" s="29"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14" t="s">
+      <c r="L17" s="46"/>
+    </row>
+    <row r="18" ht="15" spans="1:12">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D18" s="39">
         <v>25</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E18" s="40">
         <v>30</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F18" s="39">
         <v>50</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G18" s="41">
         <v>50</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H18" s="40">
         <v>46</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I18" s="41">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" ht="15.75" spans="1:9">
-      <c r="A17" s="29"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="18">
-        <v>22</v>
-      </c>
-      <c r="E17" s="18">
-        <v>35</v>
-      </c>
-      <c r="F17" s="32">
-        <v>50</v>
-      </c>
-      <c r="G17" s="33">
-        <v>50</v>
-      </c>
-      <c r="H17" s="18">
-        <v>50</v>
-      </c>
-      <c r="I17" s="33">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" ht="15" spans="1:9">
-      <c r="A18" s="29"/>
-      <c r="B18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="10">
-        <v>7</v>
-      </c>
-      <c r="E18" s="10">
-        <v>6</v>
-      </c>
-      <c r="F18" s="27">
-        <v>6</v>
-      </c>
-      <c r="G18" s="28">
-        <v>5</v>
-      </c>
-      <c r="H18" s="10">
-        <v>6</v>
-      </c>
-      <c r="I18" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" ht="15" spans="1:9">
-      <c r="A19" s="29"/>
+      <c r="L18" s="46"/>
+    </row>
+    <row r="19" ht="15" spans="1:12">
+      <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="3">
-        <v>6</v>
-      </c>
-      <c r="E19" s="3">
-        <v>7</v>
-      </c>
-      <c r="F19" s="30">
-        <v>4</v>
-      </c>
-      <c r="G19" s="31">
-        <v>4</v>
-      </c>
-      <c r="H19" s="3">
-        <v>4</v>
-      </c>
-      <c r="I19" s="31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" spans="1:9">
-      <c r="A20" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="D19" s="39">
+        <v>22</v>
+      </c>
+      <c r="E19" s="40">
+        <v>32</v>
+      </c>
+      <c r="F19" s="39">
+        <v>50</v>
+      </c>
+      <c r="G19" s="41">
+        <v>50</v>
+      </c>
+      <c r="H19" s="40">
+        <v>50</v>
+      </c>
+      <c r="I19" s="41">
+        <v>50</v>
+      </c>
+      <c r="L19" s="46"/>
+    </row>
+    <row r="20" ht="15.75" spans="1:12">
+      <c r="A20" s="12"/>
       <c r="B20" s="16"/>
       <c r="C20" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="18">
-        <v>5</v>
-      </c>
-      <c r="E20" s="18">
-        <v>7</v>
-      </c>
-      <c r="F20" s="32">
-        <v>2</v>
-      </c>
-      <c r="G20" s="33">
-        <v>2</v>
-      </c>
-      <c r="H20" s="18">
-        <v>3</v>
-      </c>
-      <c r="I20" s="33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" ht="15" spans="1:9">
-      <c r="A21" s="29"/>
-      <c r="B21" s="34" t="s">
-        <v>17</v>
+      <c r="D20" s="42">
+        <v>22</v>
+      </c>
+      <c r="E20" s="43">
+        <v>35</v>
+      </c>
+      <c r="F20" s="42">
+        <v>50</v>
+      </c>
+      <c r="G20" s="44">
+        <v>50</v>
+      </c>
+      <c r="H20" s="43">
+        <v>50</v>
+      </c>
+      <c r="I20" s="44">
+        <v>50</v>
+      </c>
+      <c r="L20" s="46"/>
+    </row>
+    <row r="21" ht="15" spans="1:12">
+      <c r="A21" s="12"/>
+      <c r="B21" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="10">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10">
-        <v>0</v>
-      </c>
-      <c r="F21" s="27">
-        <v>0</v>
-      </c>
-      <c r="G21" s="28">
-        <v>0</v>
-      </c>
-      <c r="H21" s="10">
-        <v>0</v>
-      </c>
-      <c r="I21" s="28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" ht="15" spans="1:9">
-      <c r="A22" s="29"/>
-      <c r="B22" s="35"/>
+      <c r="D21" s="39">
+        <v>7</v>
+      </c>
+      <c r="E21" s="40">
+        <v>6</v>
+      </c>
+      <c r="F21" s="39">
+        <v>6</v>
+      </c>
+      <c r="G21" s="41">
+        <v>5</v>
+      </c>
+      <c r="H21" s="40">
+        <v>6</v>
+      </c>
+      <c r="I21" s="41">
+        <v>5</v>
+      </c>
+      <c r="L21" s="46"/>
+    </row>
+    <row r="22" ht="15" spans="1:12">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="30">
-        <v>0</v>
-      </c>
-      <c r="G22" s="31">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0</v>
-      </c>
-      <c r="I22" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" spans="1:9">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="17" t="s">
+      <c r="D22" s="39">
+        <v>6</v>
+      </c>
+      <c r="E22" s="40">
+        <v>7</v>
+      </c>
+      <c r="F22" s="39">
+        <v>4</v>
+      </c>
+      <c r="G22" s="41">
+        <v>4</v>
+      </c>
+      <c r="H22" s="40">
+        <v>4</v>
+      </c>
+      <c r="I22" s="41">
+        <v>4</v>
+      </c>
+      <c r="L22" s="46"/>
+    </row>
+    <row r="23" ht="15" spans="1:12">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="39">
+        <v>5</v>
+      </c>
+      <c r="E23" s="40">
+        <v>7</v>
+      </c>
+      <c r="F23" s="39">
+        <v>2</v>
+      </c>
+      <c r="G23" s="41">
+        <v>2</v>
+      </c>
+      <c r="H23" s="40">
+        <v>3</v>
+      </c>
+      <c r="I23" s="41">
+        <v>3</v>
+      </c>
+      <c r="L23" s="46"/>
+    </row>
+    <row r="24" ht="15.75" spans="1:12">
+      <c r="A24" s="12"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="18">
-        <v>0</v>
-      </c>
-      <c r="E23" s="18">
-        <v>0</v>
-      </c>
-      <c r="F23" s="32">
-        <v>0</v>
-      </c>
-      <c r="G23" s="33">
-        <v>0</v>
-      </c>
-      <c r="H23" s="18">
-        <v>0</v>
-      </c>
-      <c r="I23" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" ht="15" spans="1:9">
-      <c r="A24" s="20" t="s">
+      <c r="D24" s="39">
+        <v>5</v>
+      </c>
+      <c r="E24" s="40">
+        <v>7</v>
+      </c>
+      <c r="F24" s="39">
+        <v>2</v>
+      </c>
+      <c r="G24" s="41">
+        <v>2</v>
+      </c>
+      <c r="H24" s="40">
+        <v>3</v>
+      </c>
+      <c r="I24" s="41">
+        <v>2</v>
+      </c>
+      <c r="L24" s="46"/>
+    </row>
+    <row r="25" ht="15" spans="1:12">
+      <c r="A25" s="12"/>
+      <c r="B25" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="36">
+        <v>0</v>
+      </c>
+      <c r="E25" s="37">
+        <v>0</v>
+      </c>
+      <c r="F25" s="36">
+        <v>0</v>
+      </c>
+      <c r="G25" s="38">
+        <v>0</v>
+      </c>
+      <c r="H25" s="37">
+        <v>0</v>
+      </c>
+      <c r="I25" s="38">
+        <v>0</v>
+      </c>
+      <c r="L25" s="46"/>
+    </row>
+    <row r="26" ht="15" spans="1:12">
+      <c r="A26" s="12"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="39">
+        <v>0</v>
+      </c>
+      <c r="E26" s="40">
+        <v>0</v>
+      </c>
+      <c r="F26" s="39">
+        <v>0</v>
+      </c>
+      <c r="G26" s="41">
+        <v>0</v>
+      </c>
+      <c r="H26" s="40">
+        <v>0</v>
+      </c>
+      <c r="I26" s="41">
+        <v>0</v>
+      </c>
+      <c r="L26" s="46"/>
+    </row>
+    <row r="27" ht="15" spans="1:12">
+      <c r="A27" s="12"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="39">
+        <v>0</v>
+      </c>
+      <c r="E27" s="40">
+        <v>0</v>
+      </c>
+      <c r="F27" s="39">
+        <v>0</v>
+      </c>
+      <c r="G27" s="41">
+        <v>0</v>
+      </c>
+      <c r="H27" s="40">
+        <v>0</v>
+      </c>
+      <c r="I27" s="41">
+        <v>0</v>
+      </c>
+      <c r="L27" s="46"/>
+    </row>
+    <row r="28" ht="15.75" spans="1:12">
+      <c r="A28" s="34"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="42">
+        <v>0</v>
+      </c>
+      <c r="E28" s="43">
+        <v>0</v>
+      </c>
+      <c r="F28" s="42">
+        <v>0</v>
+      </c>
+      <c r="G28" s="44">
+        <v>0</v>
+      </c>
+      <c r="H28" s="43">
+        <v>0</v>
+      </c>
+      <c r="I28" s="44">
+        <v>0</v>
+      </c>
+      <c r="L28" s="46"/>
+    </row>
+    <row r="29" ht="15" spans="1:12">
+      <c r="A29" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="B29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D29" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E29" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F29" s="39">
         <v>2024</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G29" s="41">
         <v>2025</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H29" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I29" s="41" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" ht="15.75" spans="1:9">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="17" t="s">
+      <c r="L29" s="46"/>
+    </row>
+    <row r="30" ht="15.75" spans="1:12">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D30" s="39">
         <v>2021</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E30" s="40">
         <v>2021</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F30" s="39">
         <v>2021</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G30" s="41">
         <v>2021</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H30" s="40">
         <v>2021</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I30" s="41">
         <v>2021</v>
       </c>
-    </row>
-    <row r="26" ht="15" spans="1:9">
-      <c r="A26" s="22"/>
-      <c r="B26" s="21" t="s">
+      <c r="L30" s="46"/>
+    </row>
+    <row r="31" ht="15" spans="1:12">
+      <c r="A31" s="22"/>
+      <c r="B31" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="36">
+        <v>57.2</v>
+      </c>
+      <c r="E31" s="37">
+        <v>58.7</v>
+      </c>
+      <c r="F31" s="36">
+        <v>8.6</v>
+      </c>
+      <c r="G31" s="38">
+        <v>9.6</v>
+      </c>
+      <c r="H31" s="37">
+        <v>27.6</v>
+      </c>
+      <c r="I31" s="38">
+        <v>29.1</v>
+      </c>
+      <c r="L31" s="46"/>
+    </row>
+    <row r="32" ht="15" spans="1:12">
+      <c r="A32" s="22"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="39">
+        <v>64.9</v>
+      </c>
+      <c r="E32" s="40">
+        <v>69.1</v>
+      </c>
+      <c r="F32" s="39">
+        <v>6</v>
+      </c>
+      <c r="G32" s="41">
+        <v>6.9</v>
+      </c>
+      <c r="H32" s="40">
+        <v>24.1</v>
+      </c>
+      <c r="I32" s="41">
+        <v>27.4</v>
+      </c>
+      <c r="L32" s="46"/>
+    </row>
+    <row r="33" ht="15" spans="1:12">
+      <c r="A33" s="22"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="39">
+        <v>72.9</v>
+      </c>
+      <c r="E33" s="40">
+        <v>84</v>
+      </c>
+      <c r="F33" s="39">
+        <v>2.5</v>
+      </c>
+      <c r="G33" s="41">
+        <v>3</v>
+      </c>
+      <c r="H33" s="40">
+        <v>11</v>
+      </c>
+      <c r="I33" s="41">
+        <v>18.8</v>
+      </c>
+      <c r="L33" s="46"/>
+    </row>
+    <row r="34" ht="15.75" spans="1:12">
+      <c r="A34" s="22"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="42">
+        <v>73.5</v>
+      </c>
+      <c r="E34" s="43">
+        <v>85.6</v>
+      </c>
+      <c r="F34" s="42">
+        <v>2.2</v>
+      </c>
+      <c r="G34" s="44">
+        <v>2.9</v>
+      </c>
+      <c r="H34" s="43">
+        <v>9</v>
+      </c>
+      <c r="I34" s="44">
+        <v>17</v>
+      </c>
+      <c r="L34" s="46"/>
+    </row>
+    <row r="35" ht="15" spans="1:12">
+      <c r="A35" s="22"/>
+      <c r="B35" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="E35" s="40">
+        <v>0.3</v>
+      </c>
+      <c r="F35" s="39">
+        <v>0</v>
+      </c>
+      <c r="G35" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="H35" s="40">
+        <v>0.1</v>
+      </c>
+      <c r="I35" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="L35" s="46"/>
+    </row>
+    <row r="36" ht="15" spans="1:12">
+      <c r="A36" s="22"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="E36" s="40">
+        <v>1</v>
+      </c>
+      <c r="F36" s="39">
+        <v>0</v>
+      </c>
+      <c r="G36" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="H36" s="40">
+        <v>0.1</v>
+      </c>
+      <c r="I36" s="41">
+        <v>0.3</v>
+      </c>
+      <c r="L36" s="46"/>
+    </row>
+    <row r="37" ht="15" spans="1:12">
+      <c r="A37" s="22"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="39">
+        <v>0.4</v>
+      </c>
+      <c r="E37" s="40">
+        <v>4</v>
+      </c>
+      <c r="F37" s="39">
+        <v>0</v>
+      </c>
+      <c r="G37" s="41">
+        <v>0</v>
+      </c>
+      <c r="H37" s="40">
+        <v>0.1</v>
+      </c>
+      <c r="I37" s="41">
+        <v>1.1</v>
+      </c>
+      <c r="L37" s="46"/>
+    </row>
+    <row r="38" ht="15.75" spans="1:12">
+      <c r="A38" s="22"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="E38" s="40">
+        <v>5.5</v>
+      </c>
+      <c r="F38" s="39">
+        <v>0</v>
+      </c>
+      <c r="G38" s="41">
+        <v>0</v>
+      </c>
+      <c r="H38" s="40">
+        <v>0</v>
+      </c>
+      <c r="I38" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="L38" s="46"/>
+    </row>
+    <row r="39" ht="15" spans="1:12">
+      <c r="A39" s="22"/>
+      <c r="B39" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C39" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="36">
+        <v>69.5</v>
+      </c>
+      <c r="E39" s="37">
+        <v>74</v>
+      </c>
+      <c r="F39" s="36">
+        <v>16.2</v>
+      </c>
+      <c r="G39" s="38">
+        <v>17.5</v>
+      </c>
+      <c r="H39" s="37">
+        <v>31.9</v>
+      </c>
+      <c r="I39" s="38">
+        <v>31.9</v>
+      </c>
+      <c r="L39" s="46"/>
+    </row>
+    <row r="40" ht="15" spans="1:12">
+      <c r="A40" s="22"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="39">
+        <v>75</v>
+      </c>
+      <c r="E40" s="40">
+        <v>80.3</v>
+      </c>
+      <c r="F40" s="39">
+        <v>16.2</v>
+      </c>
+      <c r="G40" s="41">
+        <v>17.5</v>
+      </c>
+      <c r="H40" s="40">
+        <v>31.9</v>
+      </c>
+      <c r="I40" s="41">
+        <v>31.9</v>
+      </c>
+      <c r="L40" s="46"/>
+    </row>
+    <row r="41" ht="15" spans="1:12">
+      <c r="A41" s="22"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="39">
+        <v>74.9</v>
+      </c>
+      <c r="E41" s="40">
+        <v>85.5</v>
+      </c>
+      <c r="F41" s="39">
+        <v>3</v>
+      </c>
+      <c r="G41" s="41">
+        <v>3.8</v>
+      </c>
+      <c r="H41" s="40">
+        <v>12.1</v>
+      </c>
+      <c r="I41" s="41">
+        <v>20.2</v>
+      </c>
+      <c r="L41" s="46"/>
+    </row>
+    <row r="42" ht="15.75" spans="1:12">
+      <c r="A42" s="22"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="3">
-        <v>76</v>
-      </c>
-      <c r="E26" s="3">
-        <v>87</v>
-      </c>
-      <c r="F26" s="30">
-        <v>3</v>
-      </c>
-      <c r="G26" s="31">
-        <v>4</v>
-      </c>
-      <c r="H26" s="3">
-        <v>10</v>
-      </c>
-      <c r="I26" s="31">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" spans="1:9">
-      <c r="A27" s="24"/>
-      <c r="B27" s="23" t="s">
+      <c r="D42" s="42">
+        <v>76.2</v>
+      </c>
+      <c r="E42" s="43">
+        <v>87.3</v>
+      </c>
+      <c r="F42" s="42">
+        <v>2.8</v>
+      </c>
+      <c r="G42" s="44">
+        <v>4.1</v>
+      </c>
+      <c r="H42" s="43">
+        <v>10.1</v>
+      </c>
+      <c r="I42" s="44">
+        <v>17.8</v>
+      </c>
+      <c r="L42" s="46"/>
+    </row>
+    <row r="43" ht="15" spans="1:12">
+      <c r="A43" s="22"/>
+      <c r="B43" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C43" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="E43" s="40">
+        <v>0.6</v>
+      </c>
+      <c r="F43" s="39">
+        <v>0</v>
+      </c>
+      <c r="G43" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="H43" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="I43" s="41">
+        <v>0.3</v>
+      </c>
+      <c r="L43" s="46"/>
+    </row>
+    <row r="44" ht="15" spans="1:12">
+      <c r="A44" s="22"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="E44" s="40">
+        <v>2.2</v>
+      </c>
+      <c r="F44" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="G44" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="H44" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="I44" s="41">
+        <v>0.7</v>
+      </c>
+      <c r="L44" s="46"/>
+    </row>
+    <row r="45" ht="15" spans="1:12">
+      <c r="A45" s="22"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="39">
+        <v>0.8</v>
+      </c>
+      <c r="E45" s="40">
+        <v>5.1</v>
+      </c>
+      <c r="F45" s="39">
+        <v>0</v>
+      </c>
+      <c r="G45" s="41">
+        <v>0</v>
+      </c>
+      <c r="H45" s="40">
+        <v>0.1</v>
+      </c>
+      <c r="I45" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="L45" s="46"/>
+    </row>
+    <row r="46" ht="15.75" spans="1:12">
+      <c r="A46" s="24"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="18">
-        <v>1</v>
-      </c>
-      <c r="E27" s="18">
-        <v>7</v>
-      </c>
-      <c r="F27" s="32">
-        <v>0</v>
-      </c>
-      <c r="G27" s="33">
-        <v>0</v>
-      </c>
-      <c r="H27" s="18">
-        <v>0</v>
-      </c>
-      <c r="I27" s="33">
-        <v>1</v>
-      </c>
+      <c r="D46" s="42">
+        <v>0.6</v>
+      </c>
+      <c r="E46" s="43">
+        <v>7.1</v>
+      </c>
+      <c r="F46" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="G46" s="44">
+        <v>0.3</v>
+      </c>
+      <c r="H46" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="I46" s="44">
+        <v>0.7</v>
+      </c>
+      <c r="L46" s="46"/>
+    </row>
+    <row r="47" spans="7:12">
+      <c r="G47" s="46"/>
+      <c r="L47" s="46"/>
+    </row>
+    <row r="48" spans="12:12">
+      <c r="L48" s="46"/>
+    </row>
+    <row r="49" spans="12:12">
+      <c r="L49" s="46"/>
+    </row>
+    <row r="50" spans="12:12">
+      <c r="L50" s="46"/>
+    </row>
+    <row r="51" spans="12:12">
+      <c r="L51" s="46"/>
+    </row>
+    <row r="52" spans="12:12">
+      <c r="L52" s="46"/>
+    </row>
+    <row r="53" spans="12:12">
+      <c r="L53" s="46"/>
+    </row>
+    <row r="54" spans="12:12">
+      <c r="L54" s="46"/>
+    </row>
+    <row r="55" spans="12:12">
+      <c r="L55" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A9:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A9:A28"/>
+    <mergeCell ref="A29:A46"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B46"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3437,7 +4060,7 @@
     <row r="1" ht="15" spans="1:2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" ht="13.5"/>
@@ -3503,7 +4126,7 @@
       <c r="I8" s="25"/>
     </row>
     <row r="9" ht="15" spans="1:9">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -3518,21 +4141,21 @@
       <c r="E9" s="10">
         <v>330</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="26">
         <v>467</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="27">
         <v>464</v>
       </c>
       <c r="H9" s="10">
         <v>431</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="27">
         <v>426</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:9">
-      <c r="A10" s="29"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
         <v>12</v>
@@ -3543,21 +4166,21 @@
       <c r="E10" s="3">
         <v>316</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="28">
         <v>489</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="29">
         <v>482</v>
       </c>
       <c r="H10" s="3">
         <v>458</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="29">
         <v>441</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:9">
-      <c r="A11" s="29"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17" t="s">
         <v>13</v>
@@ -3568,21 +4191,21 @@
       <c r="E11" s="18">
         <v>278</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="30">
         <v>514</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="31">
         <v>507</v>
       </c>
       <c r="H11" s="18">
         <v>506</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="31">
         <v>477</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:9">
-      <c r="A12" s="29"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -3595,21 +4218,21 @@
       <c r="E12" s="10">
         <v>0.11</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="26">
         <v>0.106</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <v>0.108</v>
       </c>
       <c r="H12" s="10">
         <v>0.096</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="27">
         <v>0.106</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:9">
-      <c r="A13" s="29"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14" t="s">
         <v>12</v>
@@ -3620,21 +4243,21 @@
       <c r="E13" s="3">
         <v>0.107</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="28">
         <v>0.112</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="29">
         <v>0.113</v>
       </c>
       <c r="H13" s="3">
         <v>0.106</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="29">
         <v>0.111</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:9">
-      <c r="A14" s="29"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="16"/>
       <c r="C14" s="17" t="s">
         <v>13</v>
@@ -3645,21 +4268,21 @@
       <c r="E14" s="18">
         <v>0.143</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="30">
         <v>0.116</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="31">
         <v>0.124</v>
       </c>
       <c r="H14" s="18">
         <v>0.115</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="31">
         <v>0.125</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:9">
-      <c r="A15" s="29"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
@@ -3672,21 +4295,21 @@
       <c r="E15" s="10">
         <v>35</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="26">
         <v>48</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="27">
         <v>51</v>
       </c>
       <c r="H15" s="10">
         <v>42</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="27">
         <v>44</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:9">
-      <c r="A16" s="29"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14" t="s">
         <v>12</v>
@@ -3697,21 +4320,21 @@
       <c r="E16" s="3">
         <v>33</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="28">
         <v>54</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="29">
         <v>54</v>
       </c>
       <c r="H16" s="3">
         <v>48</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="29">
         <v>49</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="1:9">
-      <c r="A17" s="29"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="16"/>
       <c r="C17" s="17" t="s">
         <v>13</v>
@@ -3722,21 +4345,21 @@
       <c r="E17" s="18">
         <v>37</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="30">
         <v>57</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="31">
         <v>60</v>
       </c>
       <c r="H17" s="18">
         <v>56</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="31">
         <v>57</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:9">
-      <c r="A18" s="29"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
@@ -3749,21 +4372,21 @@
       <c r="E18" s="10">
         <v>15</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="26">
         <v>20</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="27">
         <v>15</v>
       </c>
       <c r="H18" s="10">
         <v>16</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="27">
         <v>14</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:9">
-      <c r="A19" s="29"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
         <v>12</v>
@@ -3774,21 +4397,21 @@
       <c r="E19" s="3">
         <v>15</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="28">
         <v>15</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="29">
         <v>13</v>
       </c>
       <c r="H19" s="3">
         <v>13</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="29">
         <v>13</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="1:9">
-      <c r="A20" s="29"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="16"/>
       <c r="C20" s="17" t="s">
         <v>13</v>
@@ -3799,22 +4422,22 @@
       <c r="E20" s="18">
         <v>15</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="30">
         <v>11</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="31">
         <v>11</v>
       </c>
       <c r="H20" s="18">
         <v>10</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="31">
         <v>12</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:9">
-      <c r="A21" s="29"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="32" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -3826,22 +4449,22 @@
       <c r="E21" s="10">
         <v>26</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="26">
         <v>15</v>
       </c>
-      <c r="G21" s="28">
+      <c r="G21" s="27">
         <v>12</v>
       </c>
       <c r="H21" s="10">
         <v>24</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="27">
         <v>18</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:9">
-      <c r="A22" s="29"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="14" t="s">
         <v>12</v>
       </c>
@@ -3851,22 +4474,22 @@
       <c r="E22" s="3">
         <v>29</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="28">
         <v>9</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="29">
         <v>7</v>
       </c>
       <c r="H22" s="3">
         <v>18</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="29">
         <v>14</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="1:9">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="17" t="s">
         <v>13</v>
       </c>
@@ -3876,16 +4499,16 @@
       <c r="E23" s="18">
         <v>18</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="30">
         <v>3</v>
       </c>
-      <c r="G23" s="33">
+      <c r="G23" s="31">
         <v>2</v>
       </c>
       <c r="H23" s="18">
         <v>6</v>
       </c>
-      <c r="I23" s="33">
+      <c r="I23" s="31">
         <v>6</v>
       </c>
     </row>
@@ -3905,16 +4528,16 @@
       <c r="E24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="26">
         <v>2024</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="27">
         <v>2029</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="27" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3932,16 +4555,16 @@
       <c r="E25" s="18">
         <v>2021</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="30">
         <v>2021</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G25" s="31">
         <v>2021</v>
       </c>
       <c r="H25" s="18">
         <v>2021</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I25" s="31">
         <v>2021</v>
       </c>
     </row>
@@ -3959,16 +4582,16 @@
       <c r="E26" s="3">
         <v>86</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="28">
         <v>4</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G26" s="29">
         <v>6</v>
       </c>
       <c r="H26" s="3">
         <v>8</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="29">
         <v>21</v>
       </c>
     </row>
@@ -3986,16 +4609,16 @@
       <c r="E27" s="18">
         <v>6</v>
       </c>
-      <c r="F27" s="32">
-        <v>0</v>
-      </c>
-      <c r="G27" s="33">
+      <c r="F27" s="30">
+        <v>0</v>
+      </c>
+      <c r="G27" s="31">
         <v>0</v>
       </c>
       <c r="H27" s="18">
         <v>0</v>
       </c>
-      <c r="I27" s="33">
+      <c r="I27" s="31">
         <v>1</v>
       </c>
     </row>
@@ -4039,7 +4662,7 @@
     <row r="1" ht="15" spans="1:2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" ht="13.5"/>
@@ -4105,7 +4728,7 @@
       <c r="I8" s="25"/>
     </row>
     <row r="9" ht="15" spans="1:9">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -4120,21 +4743,21 @@
       <c r="E9" s="10">
         <v>347</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="26">
         <v>496</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="27">
         <v>493</v>
       </c>
       <c r="H9" s="10">
         <v>450</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="27">
         <v>453</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:9">
-      <c r="A10" s="29"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
         <v>12</v>
@@ -4145,21 +4768,21 @@
       <c r="E10" s="3">
         <v>341</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="28">
         <v>549</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="29">
         <v>545</v>
       </c>
       <c r="H10" s="3">
         <v>510</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="29">
         <v>505</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:9">
-      <c r="A11" s="29"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17" t="s">
         <v>13</v>
@@ -4170,21 +4793,21 @@
       <c r="E11" s="18">
         <v>329</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="30">
         <v>619</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="31">
         <v>620</v>
       </c>
       <c r="H11" s="18">
         <v>618</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="31">
         <v>618</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:9">
-      <c r="A12" s="29"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -4197,21 +4820,21 @@
       <c r="E12" s="10">
         <v>0.035</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="26">
         <v>0.031</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <v>0.031</v>
       </c>
       <c r="H12" s="10">
         <v>0.032</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="27">
         <v>0.032</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:9">
-      <c r="A13" s="29"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14" t="s">
         <v>12</v>
@@ -4222,21 +4845,21 @@
       <c r="E13" s="3">
         <v>0.035</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="28">
         <v>0.031</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="29">
         <v>0.031</v>
       </c>
       <c r="H13" s="3">
         <v>0.031</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="29">
         <v>0.032</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:9">
-      <c r="A14" s="29"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="16"/>
       <c r="C14" s="17" t="s">
         <v>13</v>
@@ -4247,21 +4870,21 @@
       <c r="E14" s="18">
         <v>0.043</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="30">
         <v>0.032</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="31">
         <v>0.033</v>
       </c>
       <c r="H14" s="18">
         <v>0.032</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="31">
         <v>0.033</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:9">
-      <c r="A15" s="29"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
@@ -4274,21 +4897,21 @@
       <c r="E15" s="10">
         <v>12</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="26">
         <v>15</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="27">
         <v>15</v>
       </c>
       <c r="H15" s="10">
         <v>14</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="27">
         <v>14</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:9">
-      <c r="A16" s="29"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14" t="s">
         <v>12</v>
@@ -4299,21 +4922,21 @@
       <c r="E16" s="3">
         <v>12</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="28">
         <v>17</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="29">
         <v>17</v>
       </c>
       <c r="H16" s="3">
         <v>16</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="29">
         <v>15</v>
       </c>
     </row>
     <row r="17" ht="15.75" spans="1:9">
-      <c r="A17" s="29"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="16"/>
       <c r="C17" s="17" t="s">
         <v>13</v>
@@ -4324,21 +4947,21 @@
       <c r="E17" s="18">
         <v>14</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="30">
         <v>19</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="31">
         <v>20</v>
       </c>
       <c r="H17" s="18">
         <v>19</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="31">
         <v>20</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:9">
-      <c r="A18" s="29"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
@@ -4351,21 +4974,21 @@
       <c r="E18" s="10">
         <v>1</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="26">
         <v>3</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="27">
         <v>2</v>
       </c>
       <c r="H18" s="10">
         <v>3</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:9">
-      <c r="A19" s="29"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
         <v>12</v>
@@ -4376,21 +4999,21 @@
       <c r="E19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="28">
         <v>3</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="29">
         <v>2</v>
       </c>
       <c r="H19" s="3">
         <v>2</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="29">
         <v>2</v>
       </c>
     </row>
     <row r="20" ht="15.75" spans="1:9">
-      <c r="A20" s="29"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="16"/>
       <c r="C20" s="17" t="s">
         <v>13</v>
@@ -4401,22 +5024,22 @@
       <c r="E20" s="18">
         <v>2</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="30">
         <v>2</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="31">
         <v>3</v>
       </c>
       <c r="H20" s="18">
         <v>2</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="31">
         <v>3</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:9">
-      <c r="A21" s="29"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="12"/>
+      <c r="B21" s="32" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -4428,22 +5051,22 @@
       <c r="E21" s="10">
         <v>0</v>
       </c>
-      <c r="F21" s="27">
-        <v>0</v>
-      </c>
-      <c r="G21" s="28">
+      <c r="F21" s="26">
+        <v>0</v>
+      </c>
+      <c r="G21" s="27">
         <v>0</v>
       </c>
       <c r="H21" s="10">
         <v>0</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:9">
-      <c r="A22" s="29"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="14" t="s">
         <v>12</v>
       </c>
@@ -4453,22 +5076,22 @@
       <c r="E22" s="3">
         <v>0</v>
       </c>
-      <c r="F22" s="30">
-        <v>0</v>
-      </c>
-      <c r="G22" s="31">
+      <c r="F22" s="28">
+        <v>0</v>
+      </c>
+      <c r="G22" s="29">
         <v>0</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="23" ht="15.75" spans="1:9">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="17" t="s">
         <v>13</v>
       </c>
@@ -4478,16 +5101,16 @@
       <c r="E23" s="18">
         <v>0</v>
       </c>
-      <c r="F23" s="32">
-        <v>0</v>
-      </c>
-      <c r="G23" s="33">
+      <c r="F23" s="30">
+        <v>0</v>
+      </c>
+      <c r="G23" s="31">
         <v>0</v>
       </c>
       <c r="H23" s="18">
         <v>0</v>
       </c>
-      <c r="I23" s="33">
+      <c r="I23" s="31">
         <v>0</v>
       </c>
     </row>
@@ -4507,16 +5130,16 @@
       <c r="E24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="26">
         <v>2023</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="27">
         <v>2023</v>
       </c>
       <c r="H24" s="10">
         <v>2032</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="27">
         <v>2034</v>
       </c>
     </row>
@@ -4534,16 +5157,16 @@
       <c r="E25" s="18">
         <v>2021</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="30">
         <v>2021</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G25" s="31">
         <v>2021</v>
       </c>
       <c r="H25" s="18">
         <v>2021</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I25" s="31">
         <v>2021</v>
       </c>
     </row>
@@ -4561,16 +5184,16 @@
       <c r="E26" s="3">
         <v>57</v>
       </c>
-      <c r="F26" s="30">
-        <v>0</v>
-      </c>
-      <c r="G26" s="31">
+      <c r="F26" s="28">
+        <v>0</v>
+      </c>
+      <c r="G26" s="29">
         <v>0</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="29">
         <v>1</v>
       </c>
     </row>
@@ -4588,16 +5211,16 @@
       <c r="E27" s="18">
         <v>0</v>
       </c>
-      <c r="F27" s="32">
-        <v>0</v>
-      </c>
-      <c r="G27" s="33">
+      <c r="F27" s="30">
+        <v>0</v>
+      </c>
+      <c r="G27" s="31">
         <v>0</v>
       </c>
       <c r="H27" s="18">
         <v>0</v>
       </c>
-      <c r="I27" s="33">
+      <c r="I27" s="31">
         <v>0</v>
       </c>
     </row>
@@ -4628,7 +5251,7 @@
   <sheetPr/>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:F15"/>
     </sheetView>
   </sheetViews>
@@ -4643,7 +5266,7 @@
     <row r="1" ht="15" spans="1:2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" ht="13.5"/>
@@ -4821,7 +5444,7 @@
     </row>
     <row r="18" ht="15" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>